<commit_message>
changed json data passing from excel
</commit_message>
<xml_diff>
--- a/APIAssignment/src/main/resources/TestData.xlsx
+++ b/APIAssignment/src/main/resources/TestData.xlsx
@@ -3,22 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DF2A0369-9953-442E-9690-7EF924C49DCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.lakshmi\git\RestAssured\APIAssignment\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3103936F-34A1-482E-85EB-F0FB3D9F42DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="19950" windowHeight="11700" firstSheet="4" activeTab="4" xr2:uid="{3107C3D2-330C-4DDC-B26F-7FC6C6A8C005}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="5" xr2:uid="{3107C3D2-330C-4DDC-B26F-7FC6C6A8C005}"/>
   </bookViews>
   <sheets>
     <sheet name="GetActivitiesById" sheetId="1" r:id="rId1"/>
     <sheet name="GetAuthorId" sheetId="5" r:id="rId2"/>
     <sheet name="GetBookId" sheetId="6" r:id="rId3"/>
     <sheet name="PostAuthors" sheetId="7" r:id="rId4"/>
-    <sheet name="SearchMemberResult" sheetId="9" r:id="rId5"/>
-    <sheet name="DeleteActivitiesById" sheetId="3" r:id="rId6"/>
+    <sheet name="DeleteActivitiesById" sheetId="3" r:id="rId5"/>
+    <sheet name="SearchMemberResult" sheetId="10" r:id="rId6"/>
     <sheet name="PutActivitiesById" sheetId="4" r:id="rId7"/>
     <sheet name="PostActivities" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -99,140 +103,44 @@
     <t>Last Name 3</t>
   </si>
   <si>
-    <t>subscriberID</t>
-  </si>
-  <si>
-    <t>childSearchParameter</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>columnName</t>
-  </si>
-  <si>
-    <t>sortingOrder</t>
-  </si>
-  <si>
-    <t>ASC</t>
-  </si>
-  <si>
-    <t>sortingType</t>
-  </si>
-  <si>
-    <t>ALIKE</t>
-  </si>
-  <si>
-    <t>sortOptions</t>
-  </si>
-  <si>
-    <t>pageNumber</t>
-  </si>
-  <si>
-    <t>pageOffset</t>
-  </si>
-  <si>
-    <t>subscriberIDList</t>
-  </si>
-  <si>
-    <t>planIDList</t>
-  </si>
-  <si>
-    <t>centerIDList</t>
-  </si>
-  <si>
-    <t>duration</t>
-  </si>
-  <si>
-    <t>Param1</t>
-  </si>
-  <si>
-    <t>Paramvalue1</t>
-  </si>
-  <si>
-    <t>Param2</t>
-  </si>
-  <si>
-    <t>Paramvalue2</t>
-  </si>
-  <si>
-    <t>Param3</t>
-  </si>
-  <si>
-    <t>Paramvalue3</t>
-  </si>
-  <si>
-    <t>Param4</t>
-  </si>
-  <si>
-    <t>Paramvalue4</t>
-  </si>
-  <si>
-    <t>Param5</t>
-  </si>
-  <si>
-    <t>Paramvalue5</t>
-  </si>
-  <si>
-    <t>Param6</t>
-  </si>
-  <si>
-    <t>Paramvalue6</t>
-  </si>
-  <si>
-    <t>Param7</t>
-  </si>
-  <si>
-    <t>Paramvalue7</t>
-  </si>
-  <si>
-    <t>Param8</t>
-  </si>
-  <si>
-    <t>Paramvalue8</t>
-  </si>
-  <si>
-    <t>Param9</t>
-  </si>
-  <si>
-    <t>Paramvalue9</t>
-  </si>
-  <si>
-    <t>Param10</t>
-  </si>
-  <si>
-    <t>Paramvalue10</t>
-  </si>
-  <si>
-    <t>Param11</t>
-  </si>
-  <si>
-    <t>Paramvalue11</t>
-  </si>
-  <si>
-    <t>Param12</t>
-  </si>
-  <si>
-    <t>Paramvalue12</t>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>{
+  "searchParameter": {
+    "subscriberID": "12307034"
+  },
+  "childSearchParameter": null,
+  "defaultSortOptions": [
+    {
+      "columnName": "subscriberID",
+      "sortingOrder": "ASC",
+      "sortingType": "ALIKE"
+    }
+  ],
+  "sortOptions": null,
+  "paginationOption": {
+    "pageNumber": 1,
+    "pageOffset": 50
+  },
+  "subscriberIDList": null,
+  "planIDList": null,
+  "centerIDList": null,
+  "duration" : 0
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -257,7 +165,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,172 +666,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B7C0CD-A6FA-4475-A496-39D9FEEF7B0C}">
-  <dimension ref="A1:X2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="X1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1">
-        <v>12307034</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="1">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E02780F-8C16-4ADA-ACA4-87B54A1670AA}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -949,6 +693,34 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26DFDD6-2B76-482D-AB73-E57D9D712062}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>